<commit_message>
[PHOENIX-6395] updated user name
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">juniorAssistant</t>
   </si>
   <si>
-    <t xml:space="preserve">944177</t>
+    <t xml:space="preserve">0944181</t>
   </si>
   <si>
     <t xml:space="preserve">kurnool_eGov@123</t>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">creator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944181</t>
   </si>
   <si>
     <t xml:space="preserve">deputyExecutiveEngineer</t>
@@ -297,7 +294,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,10 +332,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,19 +355,19 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +600,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -619,10 +612,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -634,7 +627,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>944162</v>
@@ -649,7 +642,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>944176</v>
@@ -664,10 +657,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
@@ -679,10 +672,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
@@ -694,10 +687,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
@@ -709,10 +702,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
@@ -724,7 +717,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>944162</v>
@@ -739,7 +732,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>27</v>
@@ -754,7 +747,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>14</v>
@@ -769,10 +762,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
@@ -784,10 +777,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -799,10 +792,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -814,7 +807,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>25</v>
@@ -829,10 +822,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -844,10 +837,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -859,10 +852,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -874,7 +867,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
@@ -889,7 +882,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>10</v>
@@ -904,7 +897,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>12</v>
@@ -919,15 +912,15 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="10" t="n">
+      <c r="D36" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -957,7 +950,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[EGSVC-30] Added the asset category UI test
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t xml:space="preserve">demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0945144</t>
   </si>
 </sst>
 </file>
@@ -218,7 +224,7 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -247,12 +253,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -325,10 +325,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -342,6 +338,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -363,21 +363,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,13 +488,13 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <f aca="false">1</f>
         <v>1</v>
       </c>
@@ -510,7 +509,7 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -525,7 +524,7 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -540,7 +539,7 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8" t="n">
+      <c r="D10" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -555,7 +554,7 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -570,7 +569,7 @@
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -585,7 +584,7 @@
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -615,7 +614,7 @@
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -624,13 +623,13 @@
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -639,13 +638,13 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="8" t="n">
         <v>944162</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -735,7 +734,7 @@
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="7" t="n">
+      <c r="D23" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -891,7 +890,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -933,6 +932,21 @@
       <c r="D36" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="10" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -957,10 +971,11 @@
     <hyperlink ref="C30" r:id="rId18" display="kurnool_eGov@123"/>
     <hyperlink ref="C31" r:id="rId19" display="kurnool_eGov@123"/>
     <hyperlink ref="C34" r:id="rId20" display="kurnool_eGov@123"/>
+    <hyperlink ref="C37" r:id="rId21" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-6396] -ui updated updated data file
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">egovernments</t>
   </si>
   <si>
     <t xml:space="preserve">assistantEngineer</t>
@@ -300,7 +303,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -338,10 +341,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -365,18 +364,19 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,22 +489,22 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="n">
-        <f aca="false">1</f>
-        <v>1</v>
+        <f aca="false">(0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>944168</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>1245501</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>944162</v>
@@ -576,10 +576,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
@@ -591,10 +591,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>5</v>
@@ -621,10 +621,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>944162</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>944176</v>
@@ -666,10 +666,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
@@ -681,10 +681,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
@@ -711,10 +711,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>944162</v>
@@ -741,10 +741,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>14</v>
@@ -771,10 +771,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
@@ -786,10 +786,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -801,10 +801,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -816,10 +816,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -831,10 +831,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -861,10 +861,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
@@ -891,10 +891,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>6</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>12</v>
@@ -921,13 +921,13 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D36" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -936,15 +936,15 @@
     </row>
     <row r="37" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="10" t="n">
+      <c r="D37" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -975,7 +975,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[EGSVC-125] UI : Completed to create the leave opening balance by using the employee id
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">0945144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hrAdmin</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -338,6 +341,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,21 +366,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,6 +951,21 @@
       <c r="D37" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="10" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -969,6 +991,7 @@
     <hyperlink ref="C31" r:id="rId19" display="kurnool_eGov@123"/>
     <hyperlink ref="C34" r:id="rId20" display="kurnool_eGov@123"/>
     <hyperlink ref="C37" r:id="rId21" display="kurnool_eGov@123"/>
+    <hyperlink ref="C38" r:id="rId22" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[EGSVC-139] UI : Completed to create the automation for employee attendance
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t xml:space="preserve">hrAdmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hrPilot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0944509</t>
   </si>
 </sst>
 </file>
@@ -303,7 +309,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -341,10 +347,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -366,21 +368,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,7 +964,22 @@
       <c r="C38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="10" t="n">
+      <c r="D38" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -992,6 +1008,7 @@
     <hyperlink ref="C34" r:id="rId20" display="kurnool_eGov@123"/>
     <hyperlink ref="C37" r:id="rId21" display="kurnool_eGov@123"/>
     <hyperlink ref="C38" r:id="rId22" display="kurnool_eGov@123"/>
+    <hyperlink ref="C39" r:id="rId23" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[PHOENIX-6503] UI : Completed only the creation of asset service for all individual categories
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t xml:space="preserve">0944509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assetCreator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0944187</t>
   </si>
 </sst>
 </file>
@@ -368,20 +374,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,6 +987,21 @@
         <v>6</v>
       </c>
       <c r="D39" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1009,6 +1031,7 @@
     <hyperlink ref="C37" r:id="rId21" display="kurnool_eGov@123"/>
     <hyperlink ref="C38" r:id="rId22" display="kurnool_eGov@123"/>
     <hyperlink ref="C39" r:id="rId23" display="kurnool_eGov@123"/>
+    <hyperlink ref="C40" r:id="rId24" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[PHOENIX-6084] UI : Modified The Approval Details in Create Agreement Screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t xml:space="preserve">assetCreator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMP0003</t>
   </si>
 </sst>
 </file>
@@ -337,6 +334,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -476,19 +474,19 @@
   </sheetPr>
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,7 +1327,7 @@
         <v>98</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
[EGSVC-32] UI : Added extra fields for Create asset screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="100">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t xml:space="preserve">assetCreator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMP0003</t>
   </si>
 </sst>
 </file>
@@ -480,13 +483,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,7 +1330,7 @@
         <v>98</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
[PHOENIX-5849] UI : Fixing Financial Tests According to the Production Data
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/loginTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t xml:space="preserve">0905867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shweta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">666666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shweta/add</t>
   </si>
   <si>
     <t xml:space="preserve">Hanuman</t>
@@ -434,11 +443,12 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -473,12 +483,6 @@
       <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -527,7 +531,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -564,10 +568,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -586,21 +586,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="18.7551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,12 +1030,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -1046,12 +1045,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1065,8 +1064,8 @@
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>55</v>
+      <c r="B31" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -1078,42 +1077,42 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="1" t="n">
@@ -1121,87 +1120,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D36" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="1" t="n">
+      <c r="B38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>6</v>
@@ -1213,10 +1212,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
@@ -1228,43 +1227,43 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="C42" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D44" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1279,7 +1278,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D45" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1291,10 +1290,10 @@
         <v>81</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D46" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1303,13 +1302,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D47" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1318,28 +1317,28 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="C48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D49" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1348,28 +1347,28 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="B51" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D51" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1378,28 +1377,28 @@
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="D52" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D53" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1410,11 +1409,11 @@
       <c r="A54" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="2" t="n">
-        <v>946800</v>
+      <c r="B54" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D54" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1423,15 +1422,15 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="B55" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="1" t="n">
+      <c r="D55" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1440,8 +1439,8 @@
       <c r="A56" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>100</v>
+      <c r="B56" s="2" t="n">
+        <v>946800</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
@@ -1453,13 +1452,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D57" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1468,13 +1467,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D58" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1483,13 +1482,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D59" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1498,13 +1497,13 @@
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="C60" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D60" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1513,13 +1512,13 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="C61" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D61" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1528,13 +1527,13 @@
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D62" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1543,13 +1542,13 @@
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="D63" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1558,13 +1557,13 @@
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D64" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1573,13 +1572,13 @@
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D65" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1588,13 +1587,13 @@
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D66" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1603,13 +1602,13 @@
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D67" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1618,13 +1617,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="D68" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1633,13 +1632,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="C69" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D69" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1648,15 +1647,45 @@
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D70" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C71" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D70" s="1" t="n">
+      <c r="D71" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1683,26 +1712,28 @@
     <hyperlink ref="C29" r:id="rId18" display="kurnool_eGov@123"/>
     <hyperlink ref="C30" r:id="rId19" display="kurnool_eGov@123"/>
     <hyperlink ref="C31" r:id="rId20" display="kurnool_eGov@123"/>
-    <hyperlink ref="C34" r:id="rId21" display="kurnool_eGov@123"/>
-    <hyperlink ref="C37" r:id="rId22" display="kurnool_eGov@123"/>
-    <hyperlink ref="C38" r:id="rId23" display="kurnool_eGov@123"/>
+    <hyperlink ref="C32" r:id="rId21" display="kurnool_eGov@123"/>
+    <hyperlink ref="C33" r:id="rId22" display="kurnool_eGov@123"/>
+    <hyperlink ref="C36" r:id="rId23" display="kurnool_eGov@123"/>
     <hyperlink ref="C39" r:id="rId24" display="kurnool_eGov@123"/>
     <hyperlink ref="C40" r:id="rId25" display="kurnool_eGov@123"/>
     <hyperlink ref="C41" r:id="rId26" display="kurnool_eGov@123"/>
-    <hyperlink ref="C53" r:id="rId27" display="kurnool_eGov@123"/>
-    <hyperlink ref="C54" r:id="rId28" display="kurnool_eGov@123"/>
+    <hyperlink ref="C42" r:id="rId27" display="kurnool_eGov@123"/>
+    <hyperlink ref="C43" r:id="rId28" display="kurnool_eGov@123"/>
     <hyperlink ref="C55" r:id="rId29" display="kurnool_eGov@123"/>
     <hyperlink ref="C56" r:id="rId30" display="kurnool_eGov@123"/>
-    <hyperlink ref="C61" r:id="rId31" display="kakinada_eGov@123"/>
-    <hyperlink ref="C62" r:id="rId32" display="kakinada_eGov@123"/>
+    <hyperlink ref="C57" r:id="rId31" display="kurnool_eGov@123"/>
+    <hyperlink ref="C58" r:id="rId32" display="kurnool_eGov@123"/>
     <hyperlink ref="C63" r:id="rId33" display="kakinada_eGov@123"/>
     <hyperlink ref="C64" r:id="rId34" display="kakinada_eGov@123"/>
     <hyperlink ref="C65" r:id="rId35" display="kakinada_eGov@123"/>
-    <hyperlink ref="C66" r:id="rId36" display="tirupati_eGov@123"/>
-    <hyperlink ref="C67" r:id="rId37" display="tirupati_eGov@123"/>
+    <hyperlink ref="C66" r:id="rId36" display="kakinada_eGov@123"/>
+    <hyperlink ref="C67" r:id="rId37" display="kakinada_eGov@123"/>
     <hyperlink ref="C68" r:id="rId38" display="tirupati_eGov@123"/>
-    <hyperlink ref="C69" r:id="rId39" display="nellore_eGov@123"/>
-    <hyperlink ref="C70" r:id="rId40" display="guntur_eGov@123"/>
+    <hyperlink ref="C69" r:id="rId39" display="tirupati_eGov@123"/>
+    <hyperlink ref="C70" r:id="rId40" display="tirupati_eGov@123"/>
+    <hyperlink ref="C71" r:id="rId41" display="nellore_eGov@123"/>
+    <hyperlink ref="C72" r:id="rId42" display="guntur_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>